<commit_message>
redesign to showProgress (2) and now is in hooks
</commit_message>
<xml_diff>
--- a/מסמכים/חישוב גביעים לניתוח אישיות והתפתחות2.xlsx
+++ b/מסמכים/חישוב גביעים לניתוח אישיות והתפתחות2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\lokchim_achraiut\progress_following\מסמכים\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA6610AD-C76B-481A-8125-A44B87425AFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33F99A9A-DA4B-4759-A8E6-CF100E4CBF8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12096" yWindow="6276" windowWidth="2388" windowHeight="564" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -372,7 +372,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -442,6 +442,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -559,7 +565,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -648,7 +654,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -682,6 +687,21 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -689,45 +709,13 @@
   </cellStyles>
   <dxfs count="9">
     <dxf>
-      <font>
-        <b/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.59999389629810485"/>
+          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -740,22 +728,36 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.59999389629810485"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -768,22 +770,16 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.59999389629810485"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -796,22 +792,16 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.59999389629810485"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0">
+      <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -824,13 +814,13 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -2115,7 +2105,7 @@
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="שם הפרק" dataDxfId="7"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="מספר הגביעים" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="גביעים משוקלל" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="גביעים משוקלל" dataDxfId="0"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="אתה בשליטה" dataDxfId="4"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="חיבור לעצמך" dataDxfId="3"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="מחוייבות להצלחה" dataDxfId="2"/>
@@ -2126,7 +2116,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="טבלה3" displayName="טבלה3" ref="A2:G33" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="טבלה3" displayName="טבלה3" ref="A2:G33" totalsRowShown="0" headerRowDxfId="5">
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="שם הפרק"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="מספר הגביעים"/>
@@ -2406,16 +2396,18 @@
   <dimension ref="A1:V36"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A34" sqref="A34"/>
+      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="8" width="7.88671875" customWidth="1"/>
+    <col min="3" max="3" width="7.88671875" customWidth="1"/>
+    <col min="4" max="4" width="7.88671875" style="8" customWidth="1"/>
+    <col min="5" max="8" width="7.88671875" style="66" customWidth="1"/>
     <col min="9" max="9" width="1.44140625" style="22" customWidth="1"/>
     <col min="10" max="10" width="8.88671875" style="22" customWidth="1"/>
     <col min="11" max="11" width="10.88671875" style="23" customWidth="1"/>
@@ -2431,34 +2423,34 @@
         <v>75</v>
       </c>
       <c r="B1" s="25"/>
-      <c r="C1" s="52" t="s">
+      <c r="C1" s="51" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
       <c r="I1" s="26"/>
-      <c r="J1" s="54" t="s">
+      <c r="J1" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="K1" s="56"/>
+      <c r="K1" s="55"/>
       <c r="L1" s="26"/>
-      <c r="M1" s="53" t="s">
+      <c r="M1" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
-      <c r="Q1" s="53"/>
+      <c r="N1" s="52"/>
+      <c r="O1" s="52"/>
+      <c r="P1" s="52"/>
+      <c r="Q1" s="52"/>
       <c r="R1" s="26"/>
-      <c r="S1" s="54" t="s">
+      <c r="S1" s="53" t="s">
         <v>42</v>
       </c>
-      <c r="T1" s="55"/>
-      <c r="U1" s="55"/>
-      <c r="V1" s="56"/>
+      <c r="T1" s="54"/>
+      <c r="U1" s="54"/>
+      <c r="V1" s="55"/>
     </row>
     <row r="2" spans="1:22" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="10" t="s">
@@ -2467,26 +2459,26 @@
       <c r="C2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="59" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="62" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="62" t="s">
         <v>11</v>
       </c>
       <c r="I2" s="21"/>
-      <c r="J2" s="57" t="s">
+      <c r="J2" s="56" t="s">
         <v>38</v>
       </c>
-      <c r="K2" s="58"/>
+      <c r="K2" s="57"/>
       <c r="L2" s="21"/>
       <c r="M2" s="17" t="s">
         <v>39</v>
@@ -2521,21 +2513,21 @@
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="45" t="s">
         <v>21</v>
       </c>
       <c r="C3" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="12">
-        <v>1</v>
-      </c>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12">
-        <v>1</v>
-      </c>
-      <c r="G3" s="12"/>
-      <c r="H3" s="12"/>
+      <c r="D3" s="42">
+        <v>1</v>
+      </c>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63">
+        <v>1</v>
+      </c>
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
       <c r="J3" s="19"/>
       <c r="K3" s="31">
         <v>1</v>
@@ -2581,21 +2573,21 @@
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" s="46" t="s">
+      <c r="B4" s="45" t="s">
         <v>45</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="12">
-        <v>1</v>
-      </c>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12">
-        <v>1</v>
-      </c>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
+      <c r="D4" s="42">
+        <v>1</v>
+      </c>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63">
+        <v>1</v>
+      </c>
+      <c r="G4" s="63"/>
+      <c r="H4" s="63"/>
       <c r="J4" s="34" t="str">
         <f>טבלה33[[#This Row],[מספר הגביעים]]</f>
         <v>זכיה אוט'</v>
@@ -2633,21 +2625,21 @@
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="45" t="s">
         <v>46</v>
       </c>
       <c r="C5" s="12">
         <v>1</v>
       </c>
-      <c r="D5" s="12">
-        <v>1</v>
-      </c>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12">
-        <v>1</v>
-      </c>
-      <c r="H5" s="12"/>
+      <c r="D5" s="42">
+        <v>1</v>
+      </c>
+      <c r="E5" s="63"/>
+      <c r="F5" s="63"/>
+      <c r="G5" s="63">
+        <v>1</v>
+      </c>
+      <c r="H5" s="63"/>
       <c r="J5" s="19"/>
       <c r="K5" s="31">
         <v>0</v>
@@ -2677,21 +2669,21 @@
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6" s="46" t="s">
+      <c r="B6" s="45" t="s">
         <v>47</v>
       </c>
       <c r="C6" s="12">
         <v>1</v>
       </c>
-      <c r="D6" s="12">
-        <v>1</v>
-      </c>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12">
-        <v>1</v>
-      </c>
-      <c r="H6" s="12"/>
+      <c r="D6" s="42">
+        <v>1</v>
+      </c>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="63">
+        <v>1</v>
+      </c>
+      <c r="H6" s="63"/>
       <c r="J6" s="19"/>
       <c r="K6" s="31">
         <v>1</v>
@@ -2721,23 +2713,23 @@
       <c r="A7">
         <v>5</v>
       </c>
-      <c r="B7" s="47" t="s">
+      <c r="B7" s="46" t="s">
         <v>48</v>
       </c>
       <c r="C7" s="12">
         <v>2</v>
       </c>
-      <c r="D7" s="12">
-        <v>2</v>
-      </c>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12">
-        <v>1</v>
-      </c>
-      <c r="G7" s="12">
-        <v>1</v>
-      </c>
-      <c r="H7" s="12"/>
+      <c r="D7" s="42">
+        <v>2</v>
+      </c>
+      <c r="E7" s="63"/>
+      <c r="F7" s="63">
+        <v>1</v>
+      </c>
+      <c r="G7" s="63">
+        <v>1</v>
+      </c>
+      <c r="H7" s="63"/>
       <c r="J7" s="19"/>
       <c r="K7" s="31">
         <v>5</v>
@@ -2767,23 +2759,23 @@
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8" s="47" t="s">
+      <c r="B8" s="46" t="s">
         <v>49</v>
       </c>
       <c r="C8" s="12">
         <v>2</v>
       </c>
-      <c r="D8" s="12">
-        <v>2</v>
-      </c>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12">
-        <v>1</v>
-      </c>
-      <c r="G8" s="12">
-        <v>1</v>
-      </c>
-      <c r="H8" s="12"/>
+      <c r="D8" s="42">
+        <v>2</v>
+      </c>
+      <c r="E8" s="63"/>
+      <c r="F8" s="63">
+        <v>1</v>
+      </c>
+      <c r="G8" s="63">
+        <v>1</v>
+      </c>
+      <c r="H8" s="63"/>
       <c r="J8" s="19"/>
       <c r="K8" s="31">
         <v>4</v>
@@ -2813,23 +2805,23 @@
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="B9" s="47" t="s">
+      <c r="B9" s="46" t="s">
         <v>50</v>
       </c>
       <c r="C9" s="12">
         <v>2</v>
       </c>
-      <c r="D9" s="12">
-        <v>2</v>
-      </c>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12">
-        <v>1</v>
-      </c>
-      <c r="G9" s="12">
+      <c r="D9" s="42">
+        <v>2</v>
+      </c>
+      <c r="E9" s="63"/>
+      <c r="F9" s="63">
+        <v>1</v>
+      </c>
+      <c r="G9" s="63">
         <v>0.5</v>
       </c>
-      <c r="H9" s="12">
+      <c r="H9" s="63">
         <v>0.5</v>
       </c>
       <c r="J9" s="19"/>
@@ -2861,23 +2853,23 @@
       <c r="A10">
         <v>8</v>
       </c>
-      <c r="B10" s="48" t="s">
+      <c r="B10" s="47" t="s">
         <v>51</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="12">
-        <v>2</v>
-      </c>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12">
-        <v>1</v>
-      </c>
-      <c r="G10" s="12">
-        <v>1</v>
-      </c>
-      <c r="H10" s="12"/>
+      <c r="D10" s="42">
+        <v>2</v>
+      </c>
+      <c r="E10" s="63"/>
+      <c r="F10" s="63">
+        <v>1</v>
+      </c>
+      <c r="G10" s="63">
+        <v>1</v>
+      </c>
+      <c r="H10" s="63"/>
       <c r="J10" s="34" t="str">
         <f>טבלה33[[#This Row],[מספר הגביעים]]</f>
         <v>זכיה אוט'</v>
@@ -2911,21 +2903,21 @@
       <c r="A11">
         <v>9</v>
       </c>
-      <c r="B11" s="48" t="s">
+      <c r="B11" s="47" t="s">
         <v>52</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="D11" s="12">
-        <v>2</v>
-      </c>
-      <c r="E11" s="12">
-        <v>2</v>
-      </c>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
+      <c r="D11" s="42">
+        <v>2</v>
+      </c>
+      <c r="E11" s="63">
+        <v>2</v>
+      </c>
+      <c r="F11" s="63"/>
+      <c r="G11" s="63"/>
+      <c r="H11" s="63"/>
       <c r="J11" s="34" t="str">
         <f>טבלה33[[#This Row],[מספר הגביעים]]</f>
         <v>זכיה אוט'</v>
@@ -2959,23 +2951,23 @@
       <c r="A12">
         <v>10</v>
       </c>
-      <c r="B12" s="48" t="s">
+      <c r="B12" s="47" t="s">
         <v>53</v>
       </c>
       <c r="C12" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="D12" s="12">
+      <c r="D12" s="42">
         <v>4</v>
       </c>
-      <c r="E12" s="12">
-        <v>1</v>
-      </c>
-      <c r="F12" s="12">
+      <c r="E12" s="63">
+        <v>1</v>
+      </c>
+      <c r="F12" s="63">
         <v>3</v>
       </c>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
+      <c r="G12" s="63"/>
+      <c r="H12" s="63"/>
       <c r="J12" s="34" t="str">
         <f>טבלה33[[#This Row],[מספר הגביעים]]</f>
         <v>זכיה אוט'</v>
@@ -3009,25 +3001,25 @@
       <c r="A13">
         <v>11</v>
       </c>
-      <c r="B13" s="49" t="s">
+      <c r="B13" s="48" t="s">
         <v>55</v>
       </c>
       <c r="C13" s="12">
         <v>14</v>
       </c>
-      <c r="D13" s="12">
+      <c r="D13" s="42">
         <v>14</v>
       </c>
-      <c r="E13" s="12">
-        <v>2</v>
-      </c>
-      <c r="F13" s="12">
-        <v>2</v>
-      </c>
-      <c r="G13" s="12">
+      <c r="E13" s="63">
+        <v>2</v>
+      </c>
+      <c r="F13" s="63">
+        <v>2</v>
+      </c>
+      <c r="G13" s="63">
         <v>5</v>
       </c>
-      <c r="H13" s="12">
+      <c r="H13" s="63">
         <v>5</v>
       </c>
       <c r="J13" s="19"/>
@@ -3059,25 +3051,25 @@
       <c r="A14">
         <v>11</v>
       </c>
-      <c r="B14" s="49" t="s">
+      <c r="B14" s="48" t="s">
         <v>54</v>
       </c>
       <c r="C14" s="12">
         <v>14</v>
       </c>
-      <c r="D14" s="12">
+      <c r="D14" s="42">
         <v>14</v>
       </c>
-      <c r="E14" s="12">
-        <v>2</v>
-      </c>
-      <c r="F14" s="12">
-        <v>2</v>
-      </c>
-      <c r="G14" s="12">
+      <c r="E14" s="63">
+        <v>2</v>
+      </c>
+      <c r="F14" s="63">
+        <v>2</v>
+      </c>
+      <c r="G14" s="63">
         <v>5</v>
       </c>
-      <c r="H14" s="12">
+      <c r="H14" s="63">
         <v>5</v>
       </c>
       <c r="J14" s="19" t="s">
@@ -3096,21 +3088,21 @@
       <c r="A15">
         <v>13</v>
       </c>
-      <c r="B15" s="48" t="s">
+      <c r="B15" s="47" t="s">
         <v>56</v>
       </c>
       <c r="C15" s="12">
         <v>2</v>
       </c>
-      <c r="D15" s="12">
-        <v>2</v>
-      </c>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12">
+      <c r="D15" s="42">
+        <v>2</v>
+      </c>
+      <c r="E15" s="63"/>
+      <c r="F15" s="63"/>
+      <c r="G15" s="63">
         <v>0.5</v>
       </c>
-      <c r="H15" s="12">
+      <c r="H15" s="63">
         <v>1.5</v>
       </c>
       <c r="J15" s="19"/>
@@ -3142,25 +3134,25 @@
       <c r="A16">
         <v>14</v>
       </c>
-      <c r="B16" s="50" t="s">
+      <c r="B16" s="49" t="s">
         <v>57</v>
       </c>
       <c r="C16" s="12">
         <v>2</v>
       </c>
-      <c r="D16" s="12">
-        <v>2</v>
-      </c>
-      <c r="E16" s="12">
+      <c r="D16" s="42">
+        <v>2</v>
+      </c>
+      <c r="E16" s="63">
         <v>0.75</v>
       </c>
-      <c r="F16" s="12">
+      <c r="F16" s="63">
         <v>0.75</v>
       </c>
-      <c r="G16" s="12">
+      <c r="G16" s="63">
         <v>0.5</v>
       </c>
-      <c r="H16" s="12"/>
+      <c r="H16" s="63"/>
       <c r="J16" s="32"/>
       <c r="K16" s="33">
         <v>0</v>
@@ -3190,23 +3182,23 @@
       <c r="A17">
         <v>15</v>
       </c>
-      <c r="B17" s="50" t="s">
+      <c r="B17" s="49" t="s">
         <v>58</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="D17" s="12">
-        <v>1</v>
-      </c>
-      <c r="E17" s="12">
+      <c r="D17" s="42">
+        <v>1</v>
+      </c>
+      <c r="E17" s="63">
         <v>0.5</v>
       </c>
-      <c r="F17" s="12">
+      <c r="F17" s="63">
         <v>0.5</v>
       </c>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
+      <c r="G17" s="63"/>
+      <c r="H17" s="63"/>
       <c r="J17" s="34" t="str">
         <f>טבלה33[[#This Row],[מספר הגביעים]]</f>
         <v>זכיה אוט'</v>
@@ -3240,23 +3232,23 @@
       <c r="A18">
         <v>16</v>
       </c>
-      <c r="B18" s="50" t="s">
+      <c r="B18" s="49" t="s">
         <v>27</v>
       </c>
       <c r="C18" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="12">
+      <c r="D18" s="42">
         <v>3</v>
       </c>
-      <c r="E18" s="12">
+      <c r="E18" s="63">
         <v>1.2</v>
       </c>
-      <c r="F18" s="12">
+      <c r="F18" s="63">
         <v>1.2</v>
       </c>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12">
+      <c r="G18" s="63"/>
+      <c r="H18" s="63">
         <v>0.6</v>
       </c>
       <c r="J18" s="34" t="str">
@@ -3292,23 +3284,23 @@
       <c r="A19">
         <v>17</v>
       </c>
-      <c r="B19" s="50" t="s">
+      <c r="B19" s="49" t="s">
         <v>59</v>
       </c>
       <c r="C19" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="D19" s="12">
+      <c r="D19" s="42">
         <v>3</v>
       </c>
-      <c r="E19" s="12">
-        <v>2</v>
-      </c>
-      <c r="F19" s="12">
-        <v>1</v>
-      </c>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
+      <c r="E19" s="63">
+        <v>2</v>
+      </c>
+      <c r="F19" s="63">
+        <v>1</v>
+      </c>
+      <c r="G19" s="63"/>
+      <c r="H19" s="63"/>
       <c r="J19" s="34" t="str">
         <f>טבלה33[[#This Row],[מספר הגביעים]]</f>
         <v>זכיה אוט'</v>
@@ -3342,25 +3334,25 @@
       <c r="A20">
         <v>18</v>
       </c>
-      <c r="B20" s="50" t="s">
+      <c r="B20" s="49" t="s">
         <v>60</v>
       </c>
       <c r="C20" s="12">
         <v>5</v>
       </c>
-      <c r="D20" s="12">
+      <c r="D20" s="42">
         <v>5</v>
       </c>
-      <c r="E20" s="12">
+      <c r="E20" s="63">
         <v>2.8</v>
       </c>
-      <c r="F20" s="12">
-        <v>1</v>
-      </c>
-      <c r="G20" s="12">
-        <v>1</v>
-      </c>
-      <c r="H20" s="12">
+      <c r="F20" s="63">
+        <v>1</v>
+      </c>
+      <c r="G20" s="63">
+        <v>1</v>
+      </c>
+      <c r="H20" s="63">
         <v>0.2</v>
       </c>
       <c r="J20" s="19"/>
@@ -3392,23 +3384,23 @@
       <c r="A21">
         <v>19</v>
       </c>
-      <c r="B21" s="50" t="s">
+      <c r="B21" s="49" t="s">
         <v>61</v>
       </c>
       <c r="C21" s="12">
         <v>2</v>
       </c>
-      <c r="D21" s="12">
-        <v>2</v>
-      </c>
-      <c r="E21" s="12">
+      <c r="D21" s="42">
+        <v>2</v>
+      </c>
+      <c r="E21" s="63">
         <v>0.9</v>
       </c>
-      <c r="F21" s="12"/>
-      <c r="G21" s="12">
+      <c r="F21" s="63"/>
+      <c r="G21" s="63">
         <v>0.2</v>
       </c>
-      <c r="H21" s="12">
+      <c r="H21" s="63">
         <v>0.9</v>
       </c>
       <c r="J21" s="19"/>
@@ -3446,15 +3438,15 @@
       <c r="C22" s="12">
         <v>1</v>
       </c>
-      <c r="D22" s="12">
+      <c r="D22" s="42">
         <v>3</v>
       </c>
-      <c r="E22" s="12"/>
-      <c r="F22" s="12"/>
-      <c r="G22" s="12">
+      <c r="E22" s="63"/>
+      <c r="F22" s="63"/>
+      <c r="G22" s="63">
         <v>3</v>
       </c>
-      <c r="H22" s="12"/>
+      <c r="H22" s="63"/>
       <c r="J22" s="19"/>
       <c r="K22" s="31">
         <v>0</v>
@@ -3490,15 +3482,15 @@
       <c r="C23" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="D23" s="12">
-        <v>2</v>
-      </c>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12">
-        <v>2</v>
-      </c>
-      <c r="H23" s="12"/>
+      <c r="D23" s="42">
+        <v>2</v>
+      </c>
+      <c r="E23" s="63"/>
+      <c r="F23" s="63"/>
+      <c r="G23" s="63">
+        <v>2</v>
+      </c>
+      <c r="H23" s="63"/>
       <c r="J23" s="34" t="str">
         <f>טבלה33[[#This Row],[מספר הגביעים]]</f>
         <v>זכיה אוט'</v>
@@ -3538,17 +3530,17 @@
       <c r="C24" s="12">
         <v>1</v>
       </c>
-      <c r="D24" s="12">
-        <v>2</v>
-      </c>
-      <c r="E24" s="12">
-        <v>1</v>
-      </c>
-      <c r="F24" s="12">
-        <v>1</v>
-      </c>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
+      <c r="D24" s="42">
+        <v>2</v>
+      </c>
+      <c r="E24" s="63">
+        <v>1</v>
+      </c>
+      <c r="F24" s="63">
+        <v>1</v>
+      </c>
+      <c r="G24" s="63"/>
+      <c r="H24" s="63"/>
       <c r="J24" s="19"/>
       <c r="K24" s="31">
         <v>0</v>
@@ -3575,15 +3567,15 @@
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B25" s="45" t="s">
+      <c r="B25" s="44" t="s">
         <v>64</v>
       </c>
       <c r="C25" s="12"/>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="12"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="63"/>
+      <c r="F25" s="63"/>
+      <c r="G25" s="63"/>
+      <c r="H25" s="63"/>
       <c r="J25" s="19"/>
       <c r="K25" s="31"/>
       <c r="M25" s="24"/>
@@ -3593,15 +3585,15 @@
       <c r="Q25" s="15"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B26" s="45" t="s">
+      <c r="B26" s="44" t="s">
         <v>65</v>
       </c>
       <c r="C26" s="12"/>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="12"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="63"/>
+      <c r="F26" s="63"/>
+      <c r="G26" s="63"/>
+      <c r="H26" s="63"/>
       <c r="J26" s="19"/>
       <c r="K26" s="31"/>
       <c r="M26" s="24"/>
@@ -3611,15 +3603,15 @@
       <c r="Q26" s="15"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B27" s="45" t="s">
+      <c r="B27" s="44" t="s">
         <v>66</v>
       </c>
       <c r="C27" s="12"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="12"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="63"/>
+      <c r="F27" s="63"/>
+      <c r="G27" s="63"/>
+      <c r="H27" s="63"/>
       <c r="J27" s="19"/>
       <c r="K27" s="31"/>
       <c r="M27" s="24"/>
@@ -3632,25 +3624,25 @@
       <c r="A28">
         <v>23</v>
       </c>
-      <c r="B28" s="45" t="s">
+      <c r="B28" s="44" t="s">
         <v>67</v>
       </c>
       <c r="C28" s="12">
         <v>10</v>
       </c>
-      <c r="D28" s="12">
+      <c r="D28" s="42">
         <v>12</v>
       </c>
-      <c r="E28" s="12">
+      <c r="E28" s="63">
         <v>3</v>
       </c>
-      <c r="F28" s="12">
+      <c r="F28" s="63">
         <v>3</v>
       </c>
-      <c r="G28" s="12">
+      <c r="G28" s="63">
         <v>3</v>
       </c>
-      <c r="H28" s="12"/>
+      <c r="H28" s="63"/>
       <c r="J28" s="19"/>
       <c r="K28" s="31">
         <v>0</v>
@@ -3677,15 +3669,15 @@
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B29" s="45" t="s">
+      <c r="B29" s="44" t="s">
         <v>68</v>
       </c>
       <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
+      <c r="D29" s="42"/>
+      <c r="E29" s="63"/>
+      <c r="F29" s="63"/>
+      <c r="G29" s="63"/>
+      <c r="H29" s="63"/>
       <c r="J29" s="19"/>
       <c r="K29" s="31"/>
       <c r="M29" s="24"/>
@@ -3698,25 +3690,25 @@
       <c r="A30">
         <v>24</v>
       </c>
-      <c r="B30" s="45" t="s">
+      <c r="B30" s="44" t="s">
         <v>69</v>
       </c>
       <c r="C30" s="12">
         <v>14</v>
       </c>
-      <c r="D30" s="12">
+      <c r="D30" s="42">
         <v>14</v>
       </c>
-      <c r="E30" s="12">
+      <c r="E30" s="63">
         <v>7</v>
       </c>
-      <c r="F30" s="12">
-        <v>2</v>
-      </c>
-      <c r="G30" s="12">
+      <c r="F30" s="63">
+        <v>2</v>
+      </c>
+      <c r="G30" s="63">
         <v>5</v>
       </c>
-      <c r="H30" s="12"/>
+      <c r="H30" s="63"/>
       <c r="J30" s="19"/>
       <c r="K30" s="31">
         <v>0</v>
@@ -3746,23 +3738,23 @@
       <c r="A31">
         <v>25</v>
       </c>
-      <c r="B31" s="45" t="s">
+      <c r="B31" s="44" t="s">
         <v>70</v>
       </c>
       <c r="C31" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="D31" s="12">
+      <c r="D31" s="42">
         <v>3</v>
       </c>
-      <c r="E31" s="12">
-        <v>1</v>
-      </c>
-      <c r="F31" s="12"/>
-      <c r="G31" s="12">
-        <v>2</v>
-      </c>
-      <c r="H31" s="12"/>
+      <c r="E31" s="63">
+        <v>1</v>
+      </c>
+      <c r="F31" s="63"/>
+      <c r="G31" s="63">
+        <v>2</v>
+      </c>
+      <c r="H31" s="63"/>
       <c r="J31" s="34" t="str">
         <f>טבלה33[[#This Row],[מספר הגביעים]]</f>
         <v>זכיה אוט'</v>
@@ -3802,17 +3794,17 @@
       <c r="C32" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="D32" s="12">
-        <v>2</v>
-      </c>
-      <c r="E32" s="12">
-        <v>1</v>
-      </c>
-      <c r="F32" s="12">
-        <v>1</v>
-      </c>
-      <c r="G32" s="12"/>
-      <c r="H32" s="12"/>
+      <c r="D32" s="42">
+        <v>2</v>
+      </c>
+      <c r="E32" s="63">
+        <v>1</v>
+      </c>
+      <c r="F32" s="63">
+        <v>1</v>
+      </c>
+      <c r="G32" s="63"/>
+      <c r="H32" s="63"/>
       <c r="J32" s="34" t="str">
         <f>טבלה33[[#This Row],[מספר הגביעים]]</f>
         <v>זכיה אוט'</v>
@@ -3852,15 +3844,15 @@
       <c r="C33" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="D33" s="12">
-        <v>2</v>
-      </c>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12">
-        <v>2</v>
-      </c>
-      <c r="G33" s="12"/>
-      <c r="H33" s="12"/>
+      <c r="D33" s="42">
+        <v>2</v>
+      </c>
+      <c r="E33" s="63"/>
+      <c r="F33" s="63">
+        <v>2</v>
+      </c>
+      <c r="G33" s="63"/>
+      <c r="H33" s="63"/>
       <c r="J33" s="34" t="str">
         <f>טבלה33[[#This Row],[מספר הגביעים]]</f>
         <v>זכיה אוט'</v>
@@ -3900,17 +3892,17 @@
       <c r="C34" s="12">
         <v>1</v>
       </c>
-      <c r="D34" s="12">
+      <c r="D34" s="42">
         <v>3</v>
       </c>
-      <c r="E34" s="12"/>
-      <c r="F34" s="12">
+      <c r="E34" s="63"/>
+      <c r="F34" s="63">
         <v>1.2</v>
       </c>
-      <c r="G34" s="12">
+      <c r="G34" s="63">
         <v>0.6</v>
       </c>
-      <c r="H34" s="12">
+      <c r="H34" s="63">
         <v>1.2</v>
       </c>
       <c r="J34" s="19"/>
@@ -3939,15 +3931,15 @@
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B35" s="51" t="s">
+      <c r="B35" s="50" t="s">
         <v>74</v>
       </c>
       <c r="C35" s="43"/>
-      <c r="D35" s="43"/>
-      <c r="E35" s="43"/>
-      <c r="F35" s="43"/>
-      <c r="G35" s="43"/>
-      <c r="H35" s="44"/>
+      <c r="D35" s="60"/>
+      <c r="E35" s="64"/>
+      <c r="F35" s="64"/>
+      <c r="G35" s="64"/>
+      <c r="H35" s="67"/>
       <c r="J35" s="19"/>
       <c r="K35" s="31"/>
       <c r="M35" s="15"/>
@@ -3961,23 +3953,23 @@
         <v>36</v>
       </c>
       <c r="C36" s="14"/>
-      <c r="D36" s="14">
+      <c r="D36" s="61">
         <f>SUM(D3:D35)-28</f>
         <v>79</v>
       </c>
-      <c r="E36" s="14">
+      <c r="E36" s="65">
         <f>SUM(E3:E35)</f>
         <v>28.15</v>
       </c>
-      <c r="F36" s="14">
+      <c r="F36" s="65">
         <f>SUM(F3:F35)</f>
         <v>27.65</v>
       </c>
-      <c r="G36" s="14">
+      <c r="G36" s="65">
         <f>SUM(G3:G35)</f>
         <v>33.300000000000004</v>
       </c>
-      <c r="H36" s="14">
+      <c r="H36" s="65">
         <f>SUM(H3:H35)</f>
         <v>14.899999999999999</v>
       </c>
@@ -4048,14 +4040,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="58" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="58"/>
     </row>
     <row r="2" spans="1:12" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">

</xml_diff>

<commit_message>
first version - test version
</commit_message>
<xml_diff>
--- a/מסמכים/חישוב גביעים לניתוח אישיות והתפתחות2.xlsx
+++ b/מסמכים/חישוב גביעים לניתוח אישיות והתפתחות2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\lokchim_achraiut\progress_following\מסמכים\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33F99A9A-DA4B-4759-A8E6-CF100E4CBF8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA1904B9-9595-41DC-88F4-F79CDC0C2E21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12096" yWindow="6276" windowWidth="2388" windowHeight="564" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="מערכת סופית" sheetId="2" r:id="rId1"/>
@@ -663,6 +663,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -687,21 +702,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -709,26 +709,10 @@
   </cellStyles>
   <dxfs count="9">
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
+      <font>
+        <b/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -817,10 +801,26 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-      </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <fill>
@@ -2105,7 +2105,7 @@
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="שם הפרק" dataDxfId="7"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="מספר הגביעים" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="גביעים משוקלל" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="גביעים משוקלל" dataDxfId="5"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="אתה בשליטה" dataDxfId="4"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="חיבור לעצמך" dataDxfId="3"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="מחוייבות להצלחה" dataDxfId="2"/>
@@ -2116,7 +2116,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="טבלה3" displayName="טבלה3" ref="A2:G33" totalsRowShown="0" headerRowDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="טבלה3" displayName="טבלה3" ref="A2:G33" totalsRowShown="0" headerRowDxfId="0">
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="שם הפרק"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="מספר הגביעים"/>
@@ -2396,10 +2396,10 @@
   <dimension ref="A1:V36"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F12" sqref="F12"/>
+      <selection pane="bottomRight" activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2407,7 +2407,7 @@
     <col min="2" max="2" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.88671875" customWidth="1"/>
     <col min="4" max="4" width="7.88671875" style="8" customWidth="1"/>
-    <col min="5" max="8" width="7.88671875" style="66" customWidth="1"/>
+    <col min="5" max="8" width="7.88671875" style="58" customWidth="1"/>
     <col min="9" max="9" width="1.44140625" style="22" customWidth="1"/>
     <col min="10" max="10" width="8.88671875" style="22" customWidth="1"/>
     <col min="11" max="11" width="10.88671875" style="23" customWidth="1"/>
@@ -2423,34 +2423,34 @@
         <v>75</v>
       </c>
       <c r="B1" s="25"/>
-      <c r="C1" s="51" t="s">
+      <c r="C1" s="60" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
       <c r="I1" s="26"/>
-      <c r="J1" s="53" t="s">
+      <c r="J1" s="62" t="s">
         <v>37</v>
       </c>
-      <c r="K1" s="55"/>
+      <c r="K1" s="64"/>
       <c r="L1" s="26"/>
-      <c r="M1" s="52" t="s">
+      <c r="M1" s="61" t="s">
         <v>41</v>
       </c>
-      <c r="N1" s="52"/>
-      <c r="O1" s="52"/>
-      <c r="P1" s="52"/>
-      <c r="Q1" s="52"/>
+      <c r="N1" s="61"/>
+      <c r="O1" s="61"/>
+      <c r="P1" s="61"/>
+      <c r="Q1" s="61"/>
       <c r="R1" s="26"/>
-      <c r="S1" s="53" t="s">
+      <c r="S1" s="62" t="s">
         <v>42</v>
       </c>
-      <c r="T1" s="54"/>
-      <c r="U1" s="54"/>
-      <c r="V1" s="55"/>
+      <c r="T1" s="63"/>
+      <c r="U1" s="63"/>
+      <c r="V1" s="64"/>
     </row>
     <row r="2" spans="1:22" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="10" t="s">
@@ -2459,26 +2459,26 @@
       <c r="C2" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="59" t="s">
+      <c r="D2" s="51" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="62" t="s">
+      <c r="E2" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="62" t="s">
+      <c r="F2" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="62" t="s">
+      <c r="G2" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="62" t="s">
+      <c r="H2" s="54" t="s">
         <v>11</v>
       </c>
       <c r="I2" s="21"/>
-      <c r="J2" s="56" t="s">
+      <c r="J2" s="65" t="s">
         <v>38</v>
       </c>
-      <c r="K2" s="57"/>
+      <c r="K2" s="66"/>
       <c r="L2" s="21"/>
       <c r="M2" s="17" t="s">
         <v>39</v>
@@ -2522,12 +2522,12 @@
       <c r="D3" s="42">
         <v>1</v>
       </c>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63">
-        <v>1</v>
-      </c>
-      <c r="G3" s="63"/>
-      <c r="H3" s="63"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55">
+        <v>1</v>
+      </c>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
       <c r="J3" s="19"/>
       <c r="K3" s="31">
         <v>1</v>
@@ -2582,12 +2582,12 @@
       <c r="D4" s="42">
         <v>1</v>
       </c>
-      <c r="E4" s="63"/>
-      <c r="F4" s="63">
-        <v>1</v>
-      </c>
-      <c r="G4" s="63"/>
-      <c r="H4" s="63"/>
+      <c r="E4" s="55"/>
+      <c r="F4" s="55">
+        <v>1</v>
+      </c>
+      <c r="G4" s="55"/>
+      <c r="H4" s="55"/>
       <c r="J4" s="34" t="str">
         <f>טבלה33[[#This Row],[מספר הגביעים]]</f>
         <v>זכיה אוט'</v>
@@ -2634,12 +2634,12 @@
       <c r="D5" s="42">
         <v>1</v>
       </c>
-      <c r="E5" s="63"/>
-      <c r="F5" s="63"/>
-      <c r="G5" s="63">
-        <v>1</v>
-      </c>
-      <c r="H5" s="63"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="55"/>
+      <c r="G5" s="55">
+        <v>1</v>
+      </c>
+      <c r="H5" s="55"/>
       <c r="J5" s="19"/>
       <c r="K5" s="31">
         <v>0</v>
@@ -2678,12 +2678,12 @@
       <c r="D6" s="42">
         <v>1</v>
       </c>
-      <c r="E6" s="63"/>
-      <c r="F6" s="63"/>
-      <c r="G6" s="63">
-        <v>1</v>
-      </c>
-      <c r="H6" s="63"/>
+      <c r="E6" s="55"/>
+      <c r="F6" s="55"/>
+      <c r="G6" s="55">
+        <v>1</v>
+      </c>
+      <c r="H6" s="55"/>
       <c r="J6" s="19"/>
       <c r="K6" s="31">
         <v>1</v>
@@ -2722,14 +2722,14 @@
       <c r="D7" s="42">
         <v>2</v>
       </c>
-      <c r="E7" s="63"/>
-      <c r="F7" s="63">
-        <v>1</v>
-      </c>
-      <c r="G7" s="63">
-        <v>1</v>
-      </c>
-      <c r="H7" s="63"/>
+      <c r="E7" s="55"/>
+      <c r="F7" s="55">
+        <v>1</v>
+      </c>
+      <c r="G7" s="55">
+        <v>1</v>
+      </c>
+      <c r="H7" s="55"/>
       <c r="J7" s="19"/>
       <c r="K7" s="31">
         <v>5</v>
@@ -2768,14 +2768,14 @@
       <c r="D8" s="42">
         <v>2</v>
       </c>
-      <c r="E8" s="63"/>
-      <c r="F8" s="63">
-        <v>1</v>
-      </c>
-      <c r="G8" s="63">
-        <v>1</v>
-      </c>
-      <c r="H8" s="63"/>
+      <c r="E8" s="55"/>
+      <c r="F8" s="55">
+        <v>1</v>
+      </c>
+      <c r="G8" s="55">
+        <v>1</v>
+      </c>
+      <c r="H8" s="55"/>
       <c r="J8" s="19"/>
       <c r="K8" s="31">
         <v>4</v>
@@ -2814,14 +2814,14 @@
       <c r="D9" s="42">
         <v>2</v>
       </c>
-      <c r="E9" s="63"/>
-      <c r="F9" s="63">
-        <v>1</v>
-      </c>
-      <c r="G9" s="63">
+      <c r="E9" s="55"/>
+      <c r="F9" s="55">
+        <v>1</v>
+      </c>
+      <c r="G9" s="55">
         <v>0.5</v>
       </c>
-      <c r="H9" s="63">
+      <c r="H9" s="55">
         <v>0.5</v>
       </c>
       <c r="J9" s="19"/>
@@ -2862,14 +2862,14 @@
       <c r="D10" s="42">
         <v>2</v>
       </c>
-      <c r="E10" s="63"/>
-      <c r="F10" s="63">
-        <v>1</v>
-      </c>
-      <c r="G10" s="63">
-        <v>1</v>
-      </c>
-      <c r="H10" s="63"/>
+      <c r="E10" s="55"/>
+      <c r="F10" s="55">
+        <v>1</v>
+      </c>
+      <c r="G10" s="55">
+        <v>1</v>
+      </c>
+      <c r="H10" s="55"/>
       <c r="J10" s="34" t="str">
         <f>טבלה33[[#This Row],[מספר הגביעים]]</f>
         <v>זכיה אוט'</v>
@@ -2912,12 +2912,12 @@
       <c r="D11" s="42">
         <v>2</v>
       </c>
-      <c r="E11" s="63">
-        <v>2</v>
-      </c>
-      <c r="F11" s="63"/>
-      <c r="G11" s="63"/>
-      <c r="H11" s="63"/>
+      <c r="E11" s="55">
+        <v>2</v>
+      </c>
+      <c r="F11" s="55"/>
+      <c r="G11" s="55"/>
+      <c r="H11" s="55"/>
       <c r="J11" s="34" t="str">
         <f>טבלה33[[#This Row],[מספר הגביעים]]</f>
         <v>זכיה אוט'</v>
@@ -2960,14 +2960,14 @@
       <c r="D12" s="42">
         <v>4</v>
       </c>
-      <c r="E12" s="63">
-        <v>1</v>
-      </c>
-      <c r="F12" s="63">
+      <c r="E12" s="55">
+        <v>1</v>
+      </c>
+      <c r="F12" s="55">
         <v>3</v>
       </c>
-      <c r="G12" s="63"/>
-      <c r="H12" s="63"/>
+      <c r="G12" s="55"/>
+      <c r="H12" s="55"/>
       <c r="J12" s="34" t="str">
         <f>טבלה33[[#This Row],[מספר הגביעים]]</f>
         <v>זכיה אוט'</v>
@@ -3010,16 +3010,16 @@
       <c r="D13" s="42">
         <v>14</v>
       </c>
-      <c r="E13" s="63">
-        <v>2</v>
-      </c>
-      <c r="F13" s="63">
-        <v>2</v>
-      </c>
-      <c r="G13" s="63">
+      <c r="E13" s="55">
+        <v>2</v>
+      </c>
+      <c r="F13" s="55">
+        <v>2</v>
+      </c>
+      <c r="G13" s="55">
         <v>5</v>
       </c>
-      <c r="H13" s="63">
+      <c r="H13" s="55">
         <v>5</v>
       </c>
       <c r="J13" s="19"/>
@@ -3060,16 +3060,16 @@
       <c r="D14" s="42">
         <v>14</v>
       </c>
-      <c r="E14" s="63">
-        <v>2</v>
-      </c>
-      <c r="F14" s="63">
-        <v>2</v>
-      </c>
-      <c r="G14" s="63">
+      <c r="E14" s="55">
+        <v>2</v>
+      </c>
+      <c r="F14" s="55">
+        <v>2</v>
+      </c>
+      <c r="G14" s="55">
         <v>5</v>
       </c>
-      <c r="H14" s="63">
+      <c r="H14" s="55">
         <v>5</v>
       </c>
       <c r="J14" s="19" t="s">
@@ -3097,12 +3097,12 @@
       <c r="D15" s="42">
         <v>2</v>
       </c>
-      <c r="E15" s="63"/>
-      <c r="F15" s="63"/>
-      <c r="G15" s="63">
+      <c r="E15" s="55"/>
+      <c r="F15" s="55"/>
+      <c r="G15" s="55">
         <v>0.5</v>
       </c>
-      <c r="H15" s="63">
+      <c r="H15" s="55">
         <v>1.5</v>
       </c>
       <c r="J15" s="19"/>
@@ -3143,16 +3143,16 @@
       <c r="D16" s="42">
         <v>2</v>
       </c>
-      <c r="E16" s="63">
+      <c r="E16" s="55">
         <v>0.75</v>
       </c>
-      <c r="F16" s="63">
+      <c r="F16" s="55">
         <v>0.75</v>
       </c>
-      <c r="G16" s="63">
+      <c r="G16" s="55">
         <v>0.5</v>
       </c>
-      <c r="H16" s="63"/>
+      <c r="H16" s="55"/>
       <c r="J16" s="32"/>
       <c r="K16" s="33">
         <v>0</v>
@@ -3191,14 +3191,14 @@
       <c r="D17" s="42">
         <v>1</v>
       </c>
-      <c r="E17" s="63">
+      <c r="E17" s="55">
         <v>0.5</v>
       </c>
-      <c r="F17" s="63">
+      <c r="F17" s="55">
         <v>0.5</v>
       </c>
-      <c r="G17" s="63"/>
-      <c r="H17" s="63"/>
+      <c r="G17" s="55"/>
+      <c r="H17" s="55"/>
       <c r="J17" s="34" t="str">
         <f>טבלה33[[#This Row],[מספר הגביעים]]</f>
         <v>זכיה אוט'</v>
@@ -3241,14 +3241,14 @@
       <c r="D18" s="42">
         <v>3</v>
       </c>
-      <c r="E18" s="63">
+      <c r="E18" s="55">
         <v>1.2</v>
       </c>
-      <c r="F18" s="63">
+      <c r="F18" s="55">
         <v>1.2</v>
       </c>
-      <c r="G18" s="63"/>
-      <c r="H18" s="63">
+      <c r="G18" s="55"/>
+      <c r="H18" s="55">
         <v>0.6</v>
       </c>
       <c r="J18" s="34" t="str">
@@ -3293,14 +3293,14 @@
       <c r="D19" s="42">
         <v>3</v>
       </c>
-      <c r="E19" s="63">
-        <v>2</v>
-      </c>
-      <c r="F19" s="63">
-        <v>1</v>
-      </c>
-      <c r="G19" s="63"/>
-      <c r="H19" s="63"/>
+      <c r="E19" s="55">
+        <v>2</v>
+      </c>
+      <c r="F19" s="55">
+        <v>1</v>
+      </c>
+      <c r="G19" s="55"/>
+      <c r="H19" s="55"/>
       <c r="J19" s="34" t="str">
         <f>טבלה33[[#This Row],[מספר הגביעים]]</f>
         <v>זכיה אוט'</v>
@@ -3343,16 +3343,16 @@
       <c r="D20" s="42">
         <v>5</v>
       </c>
-      <c r="E20" s="63">
+      <c r="E20" s="55">
         <v>2.8</v>
       </c>
-      <c r="F20" s="63">
-        <v>1</v>
-      </c>
-      <c r="G20" s="63">
-        <v>1</v>
-      </c>
-      <c r="H20" s="63">
+      <c r="F20" s="55">
+        <v>1</v>
+      </c>
+      <c r="G20" s="55">
+        <v>1</v>
+      </c>
+      <c r="H20" s="55">
         <v>0.2</v>
       </c>
       <c r="J20" s="19"/>
@@ -3393,14 +3393,14 @@
       <c r="D21" s="42">
         <v>2</v>
       </c>
-      <c r="E21" s="63">
+      <c r="E21" s="55">
         <v>0.9</v>
       </c>
-      <c r="F21" s="63"/>
-      <c r="G21" s="63">
+      <c r="F21" s="55"/>
+      <c r="G21" s="55">
         <v>0.2</v>
       </c>
-      <c r="H21" s="63">
+      <c r="H21" s="55">
         <v>0.9</v>
       </c>
       <c r="J21" s="19"/>
@@ -3441,12 +3441,12 @@
       <c r="D22" s="42">
         <v>3</v>
       </c>
-      <c r="E22" s="63"/>
-      <c r="F22" s="63"/>
-      <c r="G22" s="63">
+      <c r="E22" s="55"/>
+      <c r="F22" s="55"/>
+      <c r="G22" s="55">
         <v>3</v>
       </c>
-      <c r="H22" s="63"/>
+      <c r="H22" s="55"/>
       <c r="J22" s="19"/>
       <c r="K22" s="31">
         <v>0</v>
@@ -3485,12 +3485,12 @@
       <c r="D23" s="42">
         <v>2</v>
       </c>
-      <c r="E23" s="63"/>
-      <c r="F23" s="63"/>
-      <c r="G23" s="63">
-        <v>2</v>
-      </c>
-      <c r="H23" s="63"/>
+      <c r="E23" s="55"/>
+      <c r="F23" s="55"/>
+      <c r="G23" s="55">
+        <v>2</v>
+      </c>
+      <c r="H23" s="55"/>
       <c r="J23" s="34" t="str">
         <f>טבלה33[[#This Row],[מספר הגביעים]]</f>
         <v>זכיה אוט'</v>
@@ -3533,14 +3533,14 @@
       <c r="D24" s="42">
         <v>2</v>
       </c>
-      <c r="E24" s="63">
-        <v>1</v>
-      </c>
-      <c r="F24" s="63">
-        <v>1</v>
-      </c>
-      <c r="G24" s="63"/>
-      <c r="H24" s="63"/>
+      <c r="E24" s="55">
+        <v>1</v>
+      </c>
+      <c r="F24" s="55">
+        <v>1</v>
+      </c>
+      <c r="G24" s="55"/>
+      <c r="H24" s="55"/>
       <c r="J24" s="19"/>
       <c r="K24" s="31">
         <v>0</v>
@@ -3572,10 +3572,10 @@
       </c>
       <c r="C25" s="12"/>
       <c r="D25" s="42"/>
-      <c r="E25" s="63"/>
-      <c r="F25" s="63"/>
-      <c r="G25" s="63"/>
-      <c r="H25" s="63"/>
+      <c r="E25" s="55"/>
+      <c r="F25" s="55"/>
+      <c r="G25" s="55"/>
+      <c r="H25" s="55"/>
       <c r="J25" s="19"/>
       <c r="K25" s="31"/>
       <c r="M25" s="24"/>
@@ -3590,10 +3590,10 @@
       </c>
       <c r="C26" s="12"/>
       <c r="D26" s="42"/>
-      <c r="E26" s="63"/>
-      <c r="F26" s="63"/>
-      <c r="G26" s="63"/>
-      <c r="H26" s="63"/>
+      <c r="E26" s="55"/>
+      <c r="F26" s="55"/>
+      <c r="G26" s="55"/>
+      <c r="H26" s="55"/>
       <c r="J26" s="19"/>
       <c r="K26" s="31"/>
       <c r="M26" s="24"/>
@@ -3608,10 +3608,10 @@
       </c>
       <c r="C27" s="12"/>
       <c r="D27" s="42"/>
-      <c r="E27" s="63"/>
-      <c r="F27" s="63"/>
-      <c r="G27" s="63"/>
-      <c r="H27" s="63"/>
+      <c r="E27" s="55"/>
+      <c r="F27" s="55"/>
+      <c r="G27" s="55"/>
+      <c r="H27" s="55"/>
       <c r="J27" s="19"/>
       <c r="K27" s="31"/>
       <c r="M27" s="24"/>
@@ -3633,35 +3633,35 @@
       <c r="D28" s="42">
         <v>12</v>
       </c>
-      <c r="E28" s="63">
+      <c r="E28" s="55">
         <v>3</v>
       </c>
-      <c r="F28" s="63">
+      <c r="F28" s="55">
         <v>3</v>
       </c>
-      <c r="G28" s="63">
+      <c r="G28" s="55">
         <v>3</v>
       </c>
-      <c r="H28" s="63"/>
+      <c r="H28" s="55"/>
       <c r="J28" s="19"/>
       <c r="K28" s="31">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="M28" s="24">
         <f>K28/טבלה33[[#This Row],[מספר הגביעים]]</f>
-        <v>0</v>
+        <v>0.7</v>
       </c>
       <c r="N28" s="15">
         <f>M28*טבלה33[[#This Row],[אתה בשליטה]]</f>
-        <v>0</v>
+        <v>2.0999999999999996</v>
       </c>
       <c r="O28" s="15">
         <f>M28*טבלה33[[#This Row],[חיבור לעצמך]]</f>
-        <v>0</v>
+        <v>2.0999999999999996</v>
       </c>
       <c r="P28" s="15">
         <f>M28*טבלה33[[#This Row],[מחוייבות להצלחה]]</f>
-        <v>0</v>
+        <v>2.0999999999999996</v>
       </c>
       <c r="Q28" s="15">
         <f>M28*טבלה33[[#This Row],[מימוש עצמי]]</f>
@@ -3674,10 +3674,10 @@
       </c>
       <c r="C29" s="12"/>
       <c r="D29" s="42"/>
-      <c r="E29" s="63"/>
-      <c r="F29" s="63"/>
-      <c r="G29" s="63"/>
-      <c r="H29" s="63"/>
+      <c r="E29" s="55"/>
+      <c r="F29" s="55"/>
+      <c r="G29" s="55"/>
+      <c r="H29" s="55"/>
       <c r="J29" s="19"/>
       <c r="K29" s="31"/>
       <c r="M29" s="24"/>
@@ -3699,16 +3699,16 @@
       <c r="D30" s="42">
         <v>14</v>
       </c>
-      <c r="E30" s="63">
+      <c r="E30" s="55">
         <v>7</v>
       </c>
-      <c r="F30" s="63">
-        <v>2</v>
-      </c>
-      <c r="G30" s="63">
+      <c r="F30" s="55">
+        <v>2</v>
+      </c>
+      <c r="G30" s="55">
         <v>5</v>
       </c>
-      <c r="H30" s="63"/>
+      <c r="H30" s="55"/>
       <c r="J30" s="19"/>
       <c r="K30" s="31">
         <v>0</v>
@@ -3747,14 +3747,14 @@
       <c r="D31" s="42">
         <v>3</v>
       </c>
-      <c r="E31" s="63">
-        <v>1</v>
-      </c>
-      <c r="F31" s="63"/>
-      <c r="G31" s="63">
-        <v>2</v>
-      </c>
-      <c r="H31" s="63"/>
+      <c r="E31" s="55">
+        <v>1</v>
+      </c>
+      <c r="F31" s="55"/>
+      <c r="G31" s="55">
+        <v>2</v>
+      </c>
+      <c r="H31" s="55"/>
       <c r="J31" s="34" t="str">
         <f>טבלה33[[#This Row],[מספר הגביעים]]</f>
         <v>זכיה אוט'</v>
@@ -3797,14 +3797,14 @@
       <c r="D32" s="42">
         <v>2</v>
       </c>
-      <c r="E32" s="63">
-        <v>1</v>
-      </c>
-      <c r="F32" s="63">
-        <v>1</v>
-      </c>
-      <c r="G32" s="63"/>
-      <c r="H32" s="63"/>
+      <c r="E32" s="55">
+        <v>1</v>
+      </c>
+      <c r="F32" s="55">
+        <v>1</v>
+      </c>
+      <c r="G32" s="55"/>
+      <c r="H32" s="55"/>
       <c r="J32" s="34" t="str">
         <f>טבלה33[[#This Row],[מספר הגביעים]]</f>
         <v>זכיה אוט'</v>
@@ -3847,12 +3847,12 @@
       <c r="D33" s="42">
         <v>2</v>
       </c>
-      <c r="E33" s="63"/>
-      <c r="F33" s="63">
-        <v>2</v>
-      </c>
-      <c r="G33" s="63"/>
-      <c r="H33" s="63"/>
+      <c r="E33" s="55"/>
+      <c r="F33" s="55">
+        <v>2</v>
+      </c>
+      <c r="G33" s="55"/>
+      <c r="H33" s="55"/>
       <c r="J33" s="34" t="str">
         <f>טבלה33[[#This Row],[מספר הגביעים]]</f>
         <v>זכיה אוט'</v>
@@ -3895,14 +3895,14 @@
       <c r="D34" s="42">
         <v>3</v>
       </c>
-      <c r="E34" s="63"/>
-      <c r="F34" s="63">
+      <c r="E34" s="55"/>
+      <c r="F34" s="55">
         <v>1.2</v>
       </c>
-      <c r="G34" s="63">
+      <c r="G34" s="55">
         <v>0.6</v>
       </c>
-      <c r="H34" s="63">
+      <c r="H34" s="55">
         <v>1.2</v>
       </c>
       <c r="J34" s="19"/>
@@ -3935,11 +3935,11 @@
         <v>74</v>
       </c>
       <c r="C35" s="43"/>
-      <c r="D35" s="60"/>
-      <c r="E35" s="64"/>
-      <c r="F35" s="64"/>
-      <c r="G35" s="64"/>
-      <c r="H35" s="67"/>
+      <c r="D35" s="52"/>
+      <c r="E35" s="56"/>
+      <c r="F35" s="56"/>
+      <c r="G35" s="56"/>
+      <c r="H35" s="59"/>
       <c r="J35" s="19"/>
       <c r="K35" s="31"/>
       <c r="M35" s="15"/>
@@ -3953,23 +3953,23 @@
         <v>36</v>
       </c>
       <c r="C36" s="14"/>
-      <c r="D36" s="61">
+      <c r="D36" s="53">
         <f>SUM(D3:D35)-28</f>
         <v>79</v>
       </c>
-      <c r="E36" s="65">
+      <c r="E36" s="57">
         <f>SUM(E3:E35)</f>
         <v>28.15</v>
       </c>
-      <c r="F36" s="65">
+      <c r="F36" s="57">
         <f>SUM(F3:F35)</f>
         <v>27.65</v>
       </c>
-      <c r="G36" s="65">
+      <c r="G36" s="57">
         <f>SUM(G3:G35)</f>
         <v>33.300000000000004</v>
       </c>
-      <c r="H36" s="65">
+      <c r="H36" s="57">
         <f>SUM(H3:H35)</f>
         <v>14.899999999999999</v>
       </c>
@@ -4040,14 +4040,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="67" t="s">
         <v>35</v>
       </c>
-      <c r="C1" s="58"/>
-      <c r="D1" s="58"/>
-      <c r="E1" s="58"/>
-      <c r="F1" s="58"/>
-      <c r="G1" s="58"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+      <c r="G1" s="67"/>
     </row>
     <row r="2" spans="1:12" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">

</xml_diff>